<commit_message>
Documentação de visão, projeto e Arquitetura
</commit_message>
<xml_diff>
--- a/baklog do produto.xlsx
+++ b/baklog do produto.xlsx
@@ -24,30 +24,12 @@
     <t>PRODUTO:</t>
   </si>
   <si>
-    <t>GetCloset</t>
-  </si>
-  <si>
     <t>TELEASE:</t>
   </si>
   <si>
     <t>CARACTERISTICAS</t>
   </si>
   <si>
-    <t>Formulário</t>
-  </si>
-  <si>
-    <t>Login do sistema</t>
-  </si>
-  <si>
-    <t>Cadastrar Roupas</t>
-  </si>
-  <si>
-    <t>Visualizar Minhas Roupas</t>
-  </si>
-  <si>
-    <t>Acessar Roupas Favoritas</t>
-  </si>
-  <si>
     <t>Acessar Personal Stylist</t>
   </si>
   <si>
@@ -97,6 +79,24 @@
   </si>
   <si>
     <t>Compartilha status nas redes sociais</t>
+  </si>
+  <si>
+    <t>Calculadora_Ebeta</t>
+  </si>
+  <si>
+    <t>Somar</t>
+  </si>
+  <si>
+    <t>Subtrair</t>
+  </si>
+  <si>
+    <t>Dividir</t>
+  </si>
+  <si>
+    <t>Multiplicar</t>
+  </si>
+  <si>
+    <t>Interface</t>
   </si>
 </sst>
 </file>
@@ -273,6 +273,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,6 +300,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -305,24 +323,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:E14"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,195 +640,195 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="F2" s="16">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+        <v>22</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+        <v>23</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+        <v>4</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="16"/>
+        <v>8</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="17"/>
+        <v>9</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:7" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -844,13 +844,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:F3"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="F4:F14"/>
     <mergeCell ref="B10:E10"/>
@@ -863,6 +856,13 @@
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>